<commit_message>
Update README with project overview and add images
Expanded the README to include a detailed project overview, features, requirements, setup instructions, and credits. Added 'main_menu.png' and 'game.png' as screenshots for documentation. Updated 'docs/GdP_RED.xlsx' with new content.
</commit_message>
<xml_diff>
--- a/docs/GdP_RED.xlsx
+++ b/docs/GdP_RED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meow\Documents\GitHub\projet-red_Ashes-of-the-Forgotten-Gods\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E70CC41-2088-4E44-B45E-C9B980BA0A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBED04C-C89F-4462-BA2C-A8920ECAD125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D6C504DC-70C3-4139-99BE-4C6BBC477440}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="14">
   <si>
     <r>
       <rPr>
@@ -176,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -259,22 +259,22 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -289,13 +289,13 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -310,38 +310,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -484,51 +456,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,7 +870,7 @@
   <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,468 +885,552 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
-        <v>7</v>
+      <c r="E4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="20"/>
-      <c r="C5" s="16" t="s">
+    <row r="5" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="18"/>
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="5" t="s">
-        <v>7</v>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="21"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H7" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="4">
         <v>6</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4">
         <v>7</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H10" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4">
         <v>8</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="4">
         <v>9</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="4">
         <v>10</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H13" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="4">
         <v>11</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H14" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="4">
         <v>12</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H15" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="4">
         <v>13</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4">
         <v>14</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H17" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="4">
         <v>15</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H18" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="4">
         <v>16</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="4">
         <v>17</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H20" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="4">
         <v>18</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="E21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H21" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="4">
         <v>19</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="9"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H22" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4">
         <v>20</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H23" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="4">
         <v>21</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="E24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H24" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="4">
         <v>22</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="9"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H25" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4">
         <v>23</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H26" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4">
         <v>24</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H27" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4">
         <v>25</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H28" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4">
         <v>26</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H29" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="4">
         <v>27</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="E30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H30" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="4">
         <v>28</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H31" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="4">
         <v>29</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H32" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="4">
         <v>30</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="H33" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="4">
         <v>31</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="E34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G34" s="2"/>
-      <c r="H34" s="5" t="s">
-        <v>7</v>
+      <c r="H34" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>32</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="8" t="s">
-        <v>7</v>
+      <c r="E35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1601,15 +1651,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="038d55d5-b0c0-4428-8249-a455930d2317" xsi:nil="true"/>
@@ -1618,6 +1659,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1640,14 +1690,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E735A-67AF-402C-BD43-BF0A7610D2D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FD66D29-06A9-4143-B590-090B341E9F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1656,4 +1698,12 @@
     <ds:schemaRef ds:uri="b2c0e031-deb8-487f-af10-645cb71744c2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E735A-67AF-402C-BD43-BF0A7610D2D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>